<commit_message>
FIx Slicing & Import Excel
</commit_message>
<xml_diff>
--- a/public/excel/Template Input Data Barang Instrumen III.xlsx
+++ b/public/excel/Template Input Data Barang Instrumen III.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\hcdev-instrumen\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDBEE18-D283-4FAF-A0DD-8906C80A9131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB072E19-C7E5-45FF-8524-2128EFC2694F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>0-400</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Satuan</t>
   </si>
   <si>
-    <t>Lokasi</t>
-  </si>
-  <si>
     <t>Differential Pressure Transmitter</t>
   </si>
   <si>
@@ -87,24 +84,25 @@
     <t>EJA110E</t>
   </si>
   <si>
-    <t>(CONTOH)1234567</t>
-  </si>
-  <si>
-    <t>JANGAN DIHAPUS/DIGANTI</t>
+    <t>Contoh Pengisian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,12 +112,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,10 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -158,9 +149,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{36EF980F-5F98-4140-A716-6FFB9E4BCE6F}" name="Table4" displayName="Table4" ref="A1:K200" totalsRowShown="0">
-  <autoFilter ref="A1:K200" xr:uid="{36EF980F-5F98-4140-A716-6FFB9E4BCE6F}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{36EF980F-5F98-4140-A716-6FFB9E4BCE6F}" name="Table4" displayName="Table4" ref="A1:J200" totalsRowShown="0">
+  <autoFilter ref="A1:J200" xr:uid="{36EF980F-5F98-4140-A716-6FFB9E4BCE6F}"/>
+  <tableColumns count="10">
     <tableColumn id="2" xr3:uid="{1949F6EA-4092-4E2A-A4E8-5710F9FB550D}" name="Material Number"/>
     <tableColumn id="3" xr3:uid="{4948F796-BEB1-47F9-8A0C-A7CD2D380D26}" name="Nama Barang"/>
     <tableColumn id="4" xr3:uid="{0F7134C0-A189-449C-A98D-1D593D1B32DF}" name="Range Pengukuran"/>
@@ -171,7 +162,6 @@
     <tableColumn id="9" xr3:uid="{A575DD35-9DA1-47D8-93E5-03B3047CB661}" name="Tipe"/>
     <tableColumn id="10" xr3:uid="{CC3649F5-001A-49FE-B25E-3243889A4F55}" name="Jumlah Barang"/>
     <tableColumn id="11" xr3:uid="{4BEB14CB-87C6-41FF-AD6D-F469DB4AA344}" name="Satuan"/>
-    <tableColumn id="12" xr3:uid="{B748CE51-2120-4C9B-AE36-2B5C7897EED1}" name="Lokasi"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -464,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,11 +471,17 @@
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="49" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -516,49 +512,44 @@
       <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L2" s="1">
+        <v>1234567</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="T2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1">
+      <c r="U2" s="1">
         <v>1</v>
-      </c>
-      <c r="K2" s="1">
-        <v>3</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>